<commit_message>
Beginnning to add index validation to sample pooling.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_pooling_v3_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_pooling_v3_13_0.xlsx
@@ -2089,7 +2089,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.38"/>
@@ -3528,12 +3528,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.98"/>
@@ -5284,10 +5284,10 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.78"/>

</xml_diff>

<commit_message>
test for validate_distance_matrix. corrections to tests templates.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_pooling_v3_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_pooling_v3_13_0.xlsx
@@ -2089,7 +2089,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.38"/>
@@ -3528,7 +3528,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.67"/>
@@ -5287,7 +5287,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.78"/>
@@ -5313,7 +5313,7 @@
       <c r="E1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="45" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5333,7 +5333,7 @@
       <c r="E2" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="45" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5353,7 +5353,7 @@
       <c r="E3" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="45" t="s">
         <v>31</v>
       </c>
     </row>
@@ -5373,7 +5373,7 @@
       <c r="E4" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5393,7 +5393,7 @@
       <c r="E5" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="45" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
resolved small template issue.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_pooling_v3_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_pooling_v3_13_0.xlsx
@@ -2089,7 +2089,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.38"/>
@@ -2102,6 +2102,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,6 +2110,7 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
@@ -3528,7 +3530,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.67"/>
@@ -5287,7 +5289,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.78"/>

</xml_diff>